<commit_message>
Correcting DPE for correct variable names
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EA4E7A-6D89-4ED0-B5C5-16FEF192026C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B04E32-EF9E-4776-82D2-5C2A0B2303A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="486">
   <si>
     <t>index</t>
   </si>
@@ -1201,9 +1201,6 @@
     <t>.=missing ; .=missing</t>
   </si>
   <si>
-    <t>y8sfhealth</t>
-  </si>
-  <si>
     <t>General health</t>
   </si>
   <si>
@@ -1237,18 +1234,12 @@
     <t>Cognitive Test score</t>
   </si>
   <si>
-    <t>sleepduration</t>
-  </si>
-  <si>
     <t>Sleep duration</t>
   </si>
   <si>
     <t>hr</t>
   </si>
   <si>
-    <t>sleepquality</t>
-  </si>
-  <si>
     <t>Sleep quality</t>
   </si>
   <si>
@@ -1267,21 +1258,6 @@
     <t>idproj</t>
   </si>
   <si>
-    <t>y8q125</t>
-  </si>
-  <si>
-    <t>y8q101; y8q102</t>
-  </si>
-  <si>
-    <t>y8q102</t>
-  </si>
-  <si>
-    <t>y8q127</t>
-  </si>
-  <si>
-    <t>y8q65</t>
-  </si>
-  <si>
     <t>waistmmave</t>
   </si>
   <si>
@@ -1301,39 +1277,6 @@
   </si>
   <si>
     <t>cholesterol</t>
-  </si>
-  <si>
-    <t>hdl_Chol</t>
-  </si>
-  <si>
-    <t>ldl_Chol</t>
-  </si>
-  <si>
-    <t>cholesterol ; hdl_Chol ; triglycerides</t>
-  </si>
-  <si>
-    <t>triglycerides</t>
-  </si>
-  <si>
-    <t>y8q121</t>
-  </si>
-  <si>
-    <t>y8q122</t>
-  </si>
-  <si>
-    <t>y8q59; y8q60</t>
-  </si>
-  <si>
-    <t>y8q59</t>
-  </si>
-  <si>
-    <t>y8q55</t>
-  </si>
-  <si>
-    <t>y8q53a ; y8q53b</t>
-  </si>
-  <si>
-    <t>y8q24c; y8q24d; y8q24r</t>
   </si>
   <si>
     <t>Self-reported heart disease; _x000D_
@@ -1341,67 +1284,27 @@
 Self-reported thrombosis</t>
   </si>
   <si>
-    <t>y8q24f; y8q24g; y8q24h</t>
-  </si>
-  <si>
     <t>Self-reported osteoarthritis;_x000D_
 Self-reported rheumatoid arthritis;_x000D_
 Self-reported other arthritis</t>
   </si>
   <si>
-    <t>y8q24a; y8q24b</t>
-  </si>
-  <si>
-    <t>y8q24z; y8q24aa; y8q25; y8q27a</t>
-  </si>
-  <si>
     <t>Skin cancer; Other cancer; Cervical cancer; Breast cancer;</t>
   </si>
   <si>
-    <t>y8q27b</t>
-  </si>
-  <si>
     <t>y8cesd10</t>
-  </si>
-  <si>
-    <t>y8q64atotmins; y8q64btotmins</t>
-  </si>
-  <si>
-    <t>y8q119a</t>
   </si>
   <si>
     <t>Walking briskly_frequency. Self-reported by participants. Questions adapted from Active Australia’s 1999 National Physical Activity Survey. Question is : "Please state how many times you did each type of activity and how much time you spent altogether doing each type of activity last week: Walking briskly (for recreation or exercise, or to get from place to place). _x000D_
 (If you did not do an activity, please write “0” in the boxes)". Only count activities that lasted for 10 minutes or more; add up all the times you spent in each activity to get the total time for each activity.</t>
   </si>
   <si>
-    <t>y8q120a;_x000D_
-y8q120b</t>
-  </si>
-  <si>
     <t>LTPA_indiviudal sports; _x000D_
 LTPA_team sports</t>
   </si>
   <si>
-    <t>y8q119b; _x000D_
-y8q119c;_x000D_
-y8q120a;_x000D_
-y8q120b</t>
-  </si>
-  <si>
     <t>Moderate lesiure time activity_frequency; _x000D_
 Vigorous lesiure time activity_frequency</t>
-  </si>
-  <si>
-    <t>y8q11a;_x000D_
-y8q11b;_x000D_
-y8q11c;_x000D_
-y8q11d;_x000D_
-y8q11e;_x000D_
-y8q11f;_x000D_
-y8q11g;_x000D_
-y8q11h;_x000D_
-y8q11i;_x000D_
-y8q11j</t>
   </si>
   <si>
     <t>Health limit: vigorous activities;_x000D_
@@ -1633,16 +1536,7 @@
     <t>format(as.Date(clinicdate, format = "%d/%m/%Y"), "%Y-%m-%d")</t>
   </si>
   <si>
-    <t>case_when(_x000D_
-y8q101 %in% c(2, 3) ~ 0L;_x000D_
-y8q102 %in% 1:9 ~ 1L;_x000D_
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>ifelse(is.na(waistmmave), NA, 2)</t>
-  </si>
-  <si>
-    <t>cholesterol - hdl_Chol - (triglycerides/2.2)</t>
   </si>
   <si>
     <t>Consider 1 piece or half-cup of fruits is approximatively 80 grams. _x000D_
@@ -1653,47 +1547,7 @@
 The answers "Less than one serve" and "5 serves or more" could not be harmonized, and are equal to NA in harmonized dataset.</t>
   </si>
   <si>
-    <t>case_when(_x000D_
-!is.na(y8q53b) ~ as.integer(y8q53b);_x000D_
-!is.na(y8q53a) ~ as.integer(y8q53a)*7; _x000D_
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(_x000D_
-y8y24c == 1 ~ 1L; _x000D_
-y8q24d == 1 ~ 1L;_x000D_
-y8q24r == 1 ~ 1L;_x000D_
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(_x000D_
-y8y24f == 1 ~ 1L; _x000D_
-y8q24g == 1 ~ 1L;_x000D_
-y8q24h == 1 ~ 1L;_x000D_
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(_x000D_
-y8y24a == 1 ~ 1L; _x000D_
-y8q24b == 1 ~ 1L;_x000D_
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>The category "Other" could not pe produced.</t>
-  </si>
-  <si>
-    <t>case_when(_x000D_
-y8y24a == 1 ~ 1L; _x000D_
-y8q24b == 1 ~ 2L;_x000D_
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(_x000D_
-y8q24z == 1 ~ 1L; _x000D_
-y8q24aa == 1 ~ 1L;_x000D_
-y8q25 == 1 ~ 1L;_x000D_
-y8q27a == 1 ~ 1L;_x000D_
-ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>case_when( sleepduration &gt;= 0 &amp; sleepduration &lt; 6.25 ~ 1L;_x000D_
@@ -1708,97 +1562,247 @@
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
+    <t>recode(0=NA; 1=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>The category "No" was not produced since the information is limited to the last 3 years.</t>
+  </si>
+  <si>
+    <t>Self-reported depression. Question is " In the last 3 years have you been diagnosed or treated for depression?" Response options: Yes, No;</t>
+  </si>
+  <si>
+    <t>Self-reported Depression</t>
+  </si>
+  <si>
+    <t>recode(1=1; 2=2; 3=3; 4=3; 5=3; 6=3; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>recode(1=2; 2=1; 3=1; 4=1; 5=1; 6=1; 7=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep duration. Average sleep duration in hours derived from sleep diary. A participant reported the time they felt asleep and the time they got out of bed for 8 days using the sleep diary. This variable represents the average sleep duration for these days days. 
+</t>
+  </si>
+  <si>
+    <t>y8Q125</t>
+  </si>
+  <si>
+    <t>y8Q101; y8Q102</t>
+  </si>
+  <si>
+    <t>case_when(_x000D_
+y8Q101 %in% c(2, 3) ~ 0L;_x000D_
+y8Q102 %in% 1:9 ~ 1L;_x000D_
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q102</t>
+  </si>
+  <si>
+    <t>y8Q127</t>
+  </si>
+  <si>
+    <t>y8Q65</t>
+  </si>
+  <si>
+    <t>y8Q121</t>
+  </si>
+  <si>
+    <t>y8Q122</t>
+  </si>
+  <si>
+    <t>y8Q59; y8Q60</t>
+  </si>
+  <si>
+    <t>y8Q59</t>
+  </si>
+  <si>
+    <t>y8Q55</t>
+  </si>
+  <si>
+    <t>y8Q53a ; y8Q53b</t>
+  </si>
+  <si>
+    <t>case_when(_x000D_
+!is.na(y8Q53b) ~ as.integer(y8Q53b);_x000D_
+!is.na(y8Q53a) ~ as.integer(y8Q53a)*7; _x000D_
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q24c; y8Q24d; y8Q24r</t>
+  </si>
+  <si>
+    <t>y8Q24f; y8Q24g; y8Q24h</t>
+  </si>
+  <si>
+    <t>y8Q24a; y8Q24b</t>
+  </si>
+  <si>
+    <t>y8Q24z; y8Q24aa; y8Q25; y8Q27a</t>
+  </si>
+  <si>
+    <t>case_when(_x000D_
+y8Q24z == 1 ~ 1L; _x000D_
+y8Q24aa == 1 ~ 1L;_x000D_
+y8Q25 == 1 ~ 1L;_x000D_
+y8Q27a == 1 ~ 1L;_x000D_
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q27b</t>
+  </si>
+  <si>
+    <t>y8Q24m</t>
+  </si>
+  <si>
+    <t>y8Q64atotmins; y8Q64btotmins</t>
+  </si>
+  <si>
     <t>rowSums(mutate(.,_x000D_
-temp_y8q64atotmins = y8q64atotmins*5,_x000D_
-temp_y8q64btotmins = y8q64btotmins*2) %&gt;%_x000D_
-select(temp_y8q64atotmins, temp_y8q64btotmins),_x000D_
+temp_y8Q64atotmins = y8Q64atotmins*5,_x000D_
+temp_y8Q64btotmins = y8Q64btotmins*2) %&gt;%_x000D_
+select(temp_y8Q64atotmins, temp_y8Q64btotmins),_x000D_
 na.rm=TRUE) / 7 / 60</t>
   </si>
   <si>
+    <t>case_when(
+((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 == 0 ~ 0L;
+((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt; 0 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 1 ~ 1L;
+((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 1 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 3 ~ 2L;
+((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 3 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 5 ~ 3L;
+((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 5 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 7 ~ 4L;
+((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 7 ~ 5L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q119a</t>
+  </si>
+  <si>
+    <t>case_when(
+y8Q119a &gt; 1 ~ 1L;
+y8Q119a &lt;= 5 ~ 2L;
+y8Q119a &gt;= 6 ~ 3L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q120a;_x000D_
+y8Q120b</t>
+  </si>
+  <si>
+    <t>case_when(
+y8Q120a == 1 ~1L;
+y8Q120b == 1 ~ 1L;
+(y8Q120a == 0) &amp; (y8Q120b == 0) ~ 0L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q119b; _x000D_
+y8Q119c;_x000D_
+y8Q120a;_x000D_
+y8Q120b</t>
+  </si>
+  <si>
+    <t>case_when(
+(y8Q119b == 0) &amp; (y8Q119c == 0) &amp; (y8Q120a== 0) &amp; (y8Q120b== 0) ~ 0L;
+!is.na(y8Q119b) ~ 1L; 
+!is.na(y8Q119c) ~ 1L;
+y8Q120a== 1 ~ 1L;
+y8Q120b== 1 ~ 1L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>y8Q11a;_x000D_
+y8Q11b;_x000D_
+y8Q11c;_x000D_
+y8Q11d;_x000D_
+y8Q11e;_x000D_
+y8Q11f;_x000D_
+y8Q11g;_x000D_
+y8Q11h;_x000D_
+y8Q11i;_x000D_
+y8Q11j</t>
+  </si>
+  <si>
     <t>rowMeans(mutate(.,_x000D_
-temp_y8q11a = 50 * y8q11a - 50, _x000D_
-temp_y8q11b = 50 * y8q11b - 50,_x000D_
-temp_y8q11c = 50 * y8q11c - 50,_x000D_
-temp_y8q11d = 50 * y8q11d - 50,_x000D_
-temp_y8q11e = 50 * y8q11e - 50,_x000D_
-temp_y8q11f = 50 * y8q11f - 50,_x000D_
-temp_y8q11g = 50 * y8q11g - 50,_x000D_
-temp_y8q11h = 50 * y8q11h - 50,_x000D_
-temp_y8q11i = 50 * y8q11i - 50,_x000D_
-temp_y8q11j = 50 * y8q11j - 50) %&gt;%_x000D_
-select(temp_y8q11a, temp_y8q11b, temp_y8q11c, temp_y8q11d, temp_y8q11e,_x000D_
-temp_y8q11f, temp_y8q11g, temp_y8q11h, temp_y8q11i, temp_y8q11j), _x000D_
+temp_y8Q11a = 50 * y8Q11a - 50, _x000D_
+temp_y8Q11b = 50 * y8Q11b - 50,_x000D_
+temp_y8Q11c = 50 * y8Q11c - 50,_x000D_
+temp_y8Q11d = 50 * y8Q11d - 50,_x000D_
+temp_y8Q11e = 50 * y8Q11e - 50,_x000D_
+temp_y8Q11f = 50 * y8Q11f - 50,_x000D_
+temp_y8Q11g = 50 * y8Q11g - 50,_x000D_
+temp_y8Q11h = 50 * y8Q11h - 50,_x000D_
+temp_y8Q11i = 50 * y8Q11i - 50,_x000D_
+temp_y8Q11j = 50 * y8Q11j - 50) %&gt;%_x000D_
+select(temp_y8Q11a, temp_y8Q11b, temp_y8Q11c, temp_y8Q11d, temp_y8Q11e,_x000D_
+temp_y8Q11f, temp_y8Q11g, temp_y8Q11h, temp_y8Q11i, temp_y8Q11j), _x000D_
 na.rm = TRUE)</t>
   </si>
   <si>
     <t>rowSums(mutate(.,_x000D_
-temp_y8q11a = as.numeric(!is.na(y8q11a)), _x000D_
-temp_y8q11b = as.numeric(!is.na(y8q11b)),_x000D_
-temp_y8q11c = as.numeric(!is.na(y8q11c)),_x000D_
-temp_y8q11d = as.numeric(!is.na(y8q11d)),_x000D_
-temp_y8q11e = as.numeric(!is.na(y8q11e)),_x000D_
-temp_y8q11f = as.numeric(!is.na(y8q11f)),_x000D_
-temp_y8q11g = as.numeric(!is.na(y8q11g)),_x000D_
-temp_y8q11h = as.numeric(!is.na(y8q11h)),_x000D_
-temp_y8q11i = as.numeric(!is.na(y8q11i)),_x000D_
-temp_y8q11j = as.numeric(!is.na(y8q11j))) %&gt;%_x000D_
-select(temp_y8q11a, temp_y8q11b, temp_y8q11c, temp_y8q11d, temp_y8q11e,_x000D_
-temp_y8q11f, temp_y8q11g, temp_y8q11h, temp_y8q11i, temp_y8q11j), _x000D_
+temp_y8Q11a = as.numeric(!is.na(y8Q11a)), _x000D_
+temp_y8Q11b = as.numeric(!is.na(y8Q11b)),_x000D_
+temp_y8Q11c = as.numeric(!is.na(y8Q11c)),_x000D_
+temp_y8Q11d = as.numeric(!is.na(y8Q11d)),_x000D_
+temp_y8Q11e = as.numeric(!is.na(y8Q11e)),_x000D_
+temp_y8Q11f = as.numeric(!is.na(y8Q11f)),_x000D_
+temp_y8Q11g = as.numeric(!is.na(y8Q11g)),_x000D_
+temp_y8Q11h = as.numeric(!is.na(y8Q11h)),_x000D_
+temp_y8Q11i = as.numeric(!is.na(y8Q11i)),_x000D_
+temp_y8Q11j = as.numeric(!is.na(y8Q11j))) %&gt;%_x000D_
+select(temp_y8Q11a, temp_y8Q11b, temp_y8Q11c, temp_y8Q11d, temp_y8Q11e,_x000D_
+temp_y8Q11f, temp_y8Q11g, temp_y8Q11h, temp_y8Q11i, temp_y8Q11j), _x000D_
 na.rm = TRUE)</t>
   </si>
   <si>
-    <t>recode(0=NA; 1=1; ELSE=NA)</t>
-  </si>
-  <si>
-    <t>The category "No" was not produced since the information is limited to the last 3 years.</t>
-  </si>
-  <si>
-    <t>Self-reported depression. Question is " In the last 3 years have you been diagnosed or treated for depression?" Response options: Yes, No;</t>
-  </si>
-  <si>
-    <t>Self-reported Depression</t>
-  </si>
-  <si>
-    <t>y8q24m</t>
-  </si>
-  <si>
-    <t>recode(1=1; 2=2; 3=3; 4=3; 5=3; 6=3; ELSE=NA)</t>
-  </si>
-  <si>
-    <t>recode(1=2; 2=1; 3=1; 4=1; 5=1; 6=1; 7=1; ELSE=NA)</t>
+    <t>hdl_chol</t>
+  </si>
+  <si>
+    <t>ldl_chol</t>
+  </si>
+  <si>
+    <t>cholesterol ; hdl_chol ; Triglycerides</t>
+  </si>
+  <si>
+    <t>cholesterol - hdl_chol - (triglycerides/2.2)</t>
+  </si>
+  <si>
+    <t>D1_sleepqual</t>
+  </si>
+  <si>
+    <t>undetermined</t>
+  </si>
+  <si>
+    <t>y8sf</t>
   </si>
   <si>
     <t>case_when(
-(y8q119b == 0) &amp; (y8q119c == 0) &amp; (y8q120a== 0) &amp; (y8q120b== 0) ~ 0L;
-!is.na(y8q119b) ~ 1L; 
-!is.na(y8q119c) ~ 1L;
-y8q120a== 1 ~ 1L;
-y8q120b== 1 ~ 1L;
+y8Q24a == 1 ~ 1L; 
+y8Q24b == 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>case_when(
-y8q120a == 1 ~1L;
-y8q120b == 1 ~ 1L;
-(y8q120a == 0) &amp; (y8q120b == 0) ~ 0L;
+y8Q24a == 1 ~ 1L; 
+y8Q24b == 1 ~ 2L;
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>case_when(
-y8q119a &gt; 1 ~ 1L;
-y8q119a &lt;= 5 ~ 2L;
-y8q119a &gt;= 6 ~ 3L;
+y8Q24f == 1 ~ 1L; 
+y8Q24g == 1 ~ 1L;
+y8Q24h == 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>case_when(
-((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 == 0 ~ 0L;
-((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt; 0 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 1 ~ 1L;
-((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 1 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 3 ~ 2L;
-((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 3 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 5 ~ 3L;
-((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 5 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 7 ~ 4L;
-((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 7 ~ 5L;
+y8Q24c == 1 ~ 1L; 
+y8Q24d == 1 ~ 1L;
+y8Q24r == 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>floor(mpremage)</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1850,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1871,6 +1875,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1884,7 +1894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1921,6 +1931,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2265,10 +2278,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R82" sqref="R82"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,7 +2389,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="8"/>
       <c r="J2" s="11" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>23</v>
@@ -2399,7 +2412,7 @@
         <v>27</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -2450,7 +2463,7 @@
         <v>34</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>457</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -2542,13 +2555,13 @@
         <v>25</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>45</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -2576,7 +2589,7 @@
         <v>49</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>386</v>
+        <v>442</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>300</v>
@@ -2585,7 +2598,7 @@
         <v>301</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -2647,7 +2660,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2672,7 +2685,7 @@
         <v>60</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>387</v>
+        <v>443</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>303</v>
@@ -2681,7 +2694,7 @@
         <v>304</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>443</v>
+        <v>415</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -2695,7 +2708,7 @@
         <v>207</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -2809,16 +2822,16 @@
       <c r="H11" s="3"/>
       <c r="I11" s="8"/>
       <c r="J11" s="11" t="s">
-        <v>388</v>
+        <v>445</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>305</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>426</v>
+        <v>398</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>444</v>
+        <v>416</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -2905,7 +2918,7 @@
         <v>81</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>389</v>
+        <v>446</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>307</v>
@@ -2914,7 +2927,7 @@
         <v>308</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>445</v>
+        <v>417</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -2956,7 +2969,7 @@
         <v>85</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>389</v>
+        <v>446</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>307</v>
@@ -2965,7 +2978,7 @@
         <v>308</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>445</v>
+        <v>417</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -3007,16 +3020,16 @@
         <v>88</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>390</v>
+        <v>447</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>311</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>427</v>
+        <v>399</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>446</v>
+        <v>418</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -3030,7 +3043,7 @@
         <v>40</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>480</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3323,10 +3336,10 @@
       <c r="H21" s="3"/>
       <c r="I21" s="8"/>
       <c r="J21" s="11" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>324</v>
@@ -3376,7 +3389,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>323</v>
@@ -3401,7 +3414,7 @@
         <v>34</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>459</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -3517,7 +3530,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="8"/>
       <c r="J25" s="11" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>326</v>
@@ -3570,7 +3583,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="8"/>
       <c r="J26" s="11" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>328</v>
@@ -3625,7 +3638,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
       <c r="J27" s="11" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>330</v>
@@ -3817,7 +3830,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="8"/>
       <c r="J31" s="11" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>334</v>
@@ -3870,7 +3883,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="8"/>
       <c r="J32" s="11" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>336</v>
@@ -3923,7 +3936,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>398</v>
+        <v>474</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -3976,7 +3989,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>399</v>
+        <v>475</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>340</v>
@@ -4029,7 +4042,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>400</v>
+        <v>476</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4056,7 +4069,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>460</v>
+        <v>477</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4084,7 +4097,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="8"/>
       <c r="J36" s="11" t="s">
-        <v>401</v>
+        <v>146</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>347</v>
@@ -4182,20 +4195,20 @@
       <c r="H38" s="3"/>
       <c r="I38" s="8"/>
       <c r="J38" s="11" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>349</v>
       </c>
       <c r="L38" s="11" t="s">
-        <v>428</v>
+        <v>400</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>447</v>
+        <v>419</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="11" t="s">
-        <v>461</v>
+        <v>431</v>
       </c>
       <c r="P38" s="3" t="s">
         <v>25</v>
@@ -4235,16 +4248,16 @@
         <v>158</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>349</v>
       </c>
       <c r="L39" s="11" t="s">
-        <v>428</v>
+        <v>400</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>447</v>
+        <v>419</v>
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
@@ -4258,7 +4271,7 @@
         <v>40</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>479</v>
+        <v>439</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="157.5" x14ac:dyDescent="0.25">
@@ -4286,20 +4299,20 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
       <c r="J40" s="11" t="s">
-        <v>403</v>
+        <v>449</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>351</v>
       </c>
       <c r="L40" s="11" t="s">
-        <v>429</v>
+        <v>401</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>448</v>
+        <v>420</v>
       </c>
       <c r="N40" s="3"/>
       <c r="O40" s="1" t="s">
-        <v>462</v>
+        <v>432</v>
       </c>
       <c r="P40" s="3" t="s">
         <v>25</v>
@@ -4429,7 +4442,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="8"/>
       <c r="J43" s="11" t="s">
-        <v>404</v>
+        <v>450</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>353</v>
@@ -4438,7 +4451,7 @@
         <v>354</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>449</v>
+        <v>421</v>
       </c>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
@@ -4480,7 +4493,7 @@
         <v>174</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>405</v>
+        <v>451</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>355</v>
@@ -4489,7 +4502,7 @@
         <v>356</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>450</v>
+        <v>422</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
@@ -4533,7 +4546,7 @@
         <v>178</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>406</v>
+        <v>452</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>358</v>
@@ -4542,7 +4555,7 @@
         <v>359</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>451</v>
+        <v>423</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
@@ -4584,7 +4597,7 @@
         <v>181</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>406</v>
+        <v>452</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>358</v>
@@ -4593,7 +4606,7 @@
         <v>359</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>451</v>
+        <v>423</v>
       </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
@@ -4635,13 +4648,13 @@
       <c r="H47" s="3"/>
       <c r="I47" s="8"/>
       <c r="J47" s="11" t="s">
-        <v>407</v>
+        <v>453</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>362</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>430</v>
+        <v>402</v>
       </c>
       <c r="M47" s="8" t="s">
         <v>363</v>
@@ -4658,7 +4671,7 @@
         <v>207</v>
       </c>
       <c r="S47" s="11" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -4686,16 +4699,16 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="K48" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="L48" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="L48" s="3" t="s">
-        <v>366</v>
-      </c>
       <c r="M48" s="8" t="s">
-        <v>452</v>
+        <v>424</v>
       </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
@@ -4709,7 +4722,7 @@
         <v>40</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4737,20 +4750,20 @@
         <v>191</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>408</v>
+        <v>455</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="L49" s="11" t="s">
-        <v>431</v>
+        <v>403</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="N49" s="3"/>
       <c r="O49" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>25</v>
@@ -4762,7 +4775,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>464</v>
+        <v>484</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4790,19 +4803,19 @@
         <v>191</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>410</v>
+        <v>456</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="L50" s="11" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>25</v>
@@ -4814,10 +4827,10 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4842,16 +4855,16 @@
         <v>191</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>412</v>
+        <v>457</v>
       </c>
       <c r="K51" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="L51" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="L51" s="3" t="s">
-        <v>370</v>
-      </c>
       <c r="M51" s="8" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
@@ -4865,10 +4878,10 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4893,20 +4906,20 @@
         <v>200</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>412</v>
+        <v>457</v>
       </c>
       <c r="K52" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="L52" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="L52" s="3" t="s">
-        <v>370</v>
-      </c>
       <c r="M52" s="8" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="N52" s="3"/>
       <c r="O52" s="3" t="s">
-        <v>467</v>
+        <v>433</v>
       </c>
       <c r="P52" s="3" t="s">
         <v>25</v>
@@ -4918,7 +4931,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -4946,16 +4959,16 @@
         <v>191</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>413</v>
+        <v>458</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
       <c r="L53" s="11" t="s">
-        <v>433</v>
+        <v>405</v>
       </c>
       <c r="M53" s="8" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
@@ -4969,7 +4982,7 @@
         <v>207</v>
       </c>
       <c r="S53" s="11" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
@@ -4997,16 +5010,16 @@
         <v>191</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>415</v>
+        <v>460</v>
       </c>
       <c r="K54" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="L54" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="L54" s="3" t="s">
-        <v>372</v>
-      </c>
       <c r="M54" s="8" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
@@ -5183,20 +5196,20 @@
         <v>191</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>477</v>
+        <v>438</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="M58" s="8" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="N58" s="3"/>
       <c r="O58" s="3" t="s">
-        <v>475</v>
+        <v>436</v>
       </c>
       <c r="P58" s="3" t="s">
         <v>50</v>
@@ -5208,7 +5221,7 @@
         <v>40</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>474</v>
+        <v>435</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -5277,13 +5290,13 @@
       <c r="H60" s="3"/>
       <c r="I60" s="8"/>
       <c r="J60" s="11" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L60" s="11" t="s">
-        <v>434</v>
+        <v>406</v>
       </c>
       <c r="M60" s="8" t="s">
         <v>315</v>
@@ -5498,13 +5511,13 @@
       <c r="H65" s="3"/>
       <c r="I65" s="8"/>
       <c r="J65" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="K65" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="K65" s="3" t="s">
-        <v>375</v>
-      </c>
       <c r="L65" s="11" t="s">
-        <v>435</v>
+        <v>407</v>
       </c>
       <c r="M65" s="8" t="s">
         <v>315</v>
@@ -5569,7 +5582,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5593,36 +5606,36 @@
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="8"/>
-      <c r="J67" s="11" t="s">
-        <v>376</v>
+      <c r="J67" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L67" s="11" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="M67" s="8" t="s">
         <v>315</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>25</v>
+        <v>479</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>26</v>
+        <v>479</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>45</v>
+        <v>479</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5646,33 +5659,33 @@
       <c r="I68" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="J68" s="11" t="s">
-        <v>376</v>
+      <c r="J68" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L68" s="11" t="s">
-        <v>436</v>
+        <v>408</v>
       </c>
       <c r="M68" s="8" t="s">
         <v>315</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O68" s="3"/>
       <c r="P68" s="3" t="s">
-        <v>25</v>
+        <v>479</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>50</v>
+        <v>479</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>207</v>
       </c>
       <c r="S68" s="11" t="s">
-        <v>470</v>
+        <v>434</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
@@ -5700,20 +5713,20 @@
         <v>241</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>379</v>
+        <v>478</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="L69" s="11" t="s">
-        <v>437</v>
+        <v>409</v>
       </c>
       <c r="M69" s="8" t="s">
         <v>315</v>
       </c>
       <c r="N69" s="3"/>
       <c r="O69" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="P69" s="3" t="s">
         <v>25</v>
@@ -5725,7 +5738,7 @@
         <v>40</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="51" x14ac:dyDescent="0.25">
@@ -6023,19 +6036,19 @@
       <c r="H76" s="3"/>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
-        <v>417</v>
+        <v>462</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L76" s="13" t="s">
-        <v>438</v>
+        <v>410</v>
       </c>
       <c r="M76" s="8" t="s">
         <v>315</v>
       </c>
       <c r="N76" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="O76" s="3"/>
       <c r="P76" s="3" t="s">
@@ -6048,7 +6061,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6074,19 +6087,19 @@
         <v>267</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>417</v>
+        <v>462</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L77" s="13" t="s">
-        <v>438</v>
+        <v>410</v>
       </c>
       <c r="M77" s="8" t="s">
         <v>315</v>
       </c>
       <c r="N77" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="O77" s="3"/>
       <c r="P77" s="3" t="s">
@@ -6099,7 +6112,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6127,13 +6140,13 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>418</v>
+        <v>465</v>
       </c>
       <c r="K78" s="11" t="s">
-        <v>419</v>
+        <v>394</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>439</v>
+        <v>411</v>
       </c>
       <c r="M78" s="8"/>
       <c r="N78" s="3"/>
@@ -6148,7 +6161,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6221,16 +6234,16 @@
         <v>191</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>420</v>
+        <v>467</v>
       </c>
       <c r="K80" s="11" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="L80" s="11" t="s">
-        <v>440</v>
+        <v>412</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>455</v>
+        <v>427</v>
       </c>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
@@ -6244,7 +6257,7 @@
         <v>207</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6317,13 +6330,13 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>422</v>
+        <v>469</v>
       </c>
       <c r="K82" s="11" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="L82" s="11" t="s">
-        <v>441</v>
+        <v>413</v>
       </c>
       <c r="M82" s="8" t="s">
         <v>315</v>
@@ -6340,10 +6353,10 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -6366,14 +6379,14 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
-        <v>424</v>
+        <v>471</v>
       </c>
       <c r="K83" s="11" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
       <c r="L83" s="3"/>
       <c r="M83" s="8" t="s">
-        <v>456</v>
+        <v>428</v>
       </c>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
@@ -6390,7 +6403,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="285" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -6415,14 +6428,14 @@
       <c r="H84" s="3"/>
       <c r="I84" s="8"/>
       <c r="J84" s="11" t="s">
-        <v>424</v>
+        <v>471</v>
       </c>
       <c r="K84" s="11" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
       <c r="L84" s="3"/>
       <c r="M84" s="8" t="s">
-        <v>456</v>
+        <v>428</v>
       </c>
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>

</xml_diff>

<commit_message>
Correcting a few harmo rule to fit the variable format
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B04E32-EF9E-4776-82D2-5C2A0B2303A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEA8A28-50C4-4C24-B427-5F5873787EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="487">
   <si>
     <t>index</t>
   </si>
@@ -1658,13 +1658,6 @@
     <t>y8Q64atotmins; y8Q64btotmins</t>
   </si>
   <si>
-    <t>rowSums(mutate(.,_x000D_
-temp_y8Q64atotmins = y8Q64atotmins*5,_x000D_
-temp_y8Q64btotmins = y8Q64btotmins*2) %&gt;%_x000D_
-select(temp_y8Q64atotmins, temp_y8Q64btotmins),_x000D_
-na.rm=TRUE) / 7 / 60</t>
-  </si>
-  <si>
     <t>case_when(
 ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 == 0 ~ 0L;
 ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt; 0 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 1 ~ 1L;
@@ -1803,6 +1796,16 @@
   </si>
   <si>
     <t>floor(mpremage)</t>
+  </si>
+  <si>
+    <t>round(y8cesd10)</t>
+  </si>
+  <si>
+    <t>round(rowSums(mutate(.,
+temp_y8Q64atotmins = y8Q64atotmins*5,
+temp_y8Q64btotmins = y8Q64btotmins*2) %&gt;%
+select(temp_y8Q64atotmins, temp_y8Q64btotmins),
+na.rm=TRUE) / 7 / 60)</t>
   </si>
 </sst>
 </file>
@@ -2278,10 +2281,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -3936,7 +3939,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -3989,7 +3992,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>340</v>
@@ -4042,7 +4045,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4069,7 +4072,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4699,7 +4702,7 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>364</v>
@@ -4775,7 +4778,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4827,7 +4830,7 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4878,7 +4881,7 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4931,7 +4934,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -5307,13 +5310,13 @@
         <v>25</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>45</v>
+        <v>485</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5623,16 +5626,16 @@
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
@@ -5676,10 +5679,10 @@
       </c>
       <c r="O68" s="3"/>
       <c r="P68" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>207</v>
@@ -5713,7 +5716,7 @@
         <v>241</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>377</v>
@@ -6061,7 +6064,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6112,7 +6115,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6140,7 +6143,7 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>394</v>
@@ -6161,7 +6164,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6234,7 +6237,7 @@
         <v>191</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K80" s="11" t="s">
         <v>395</v>
@@ -6257,7 +6260,7 @@
         <v>207</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6330,7 +6333,7 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>396</v>
@@ -6353,7 +6356,7 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6379,7 +6382,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K83" s="11" t="s">
         <v>397</v>
@@ -6400,7 +6403,7 @@
         <v>34</v>
       </c>
       <c r="S83" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="84" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6428,7 +6431,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="8"/>
       <c r="J84" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>397</v>
@@ -6449,7 +6452,7 @@
         <v>34</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting variable names that were incorrect
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEA8A28-50C4-4C24-B427-5F5873787EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5300495-6DAF-4721-B643-50EFAEB40EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="487">
   <si>
     <t>index</t>
   </si>
@@ -1655,19 +1655,6 @@
     <t>y8Q24m</t>
   </si>
   <si>
-    <t>y8Q64atotmins; y8Q64btotmins</t>
-  </si>
-  <si>
-    <t>case_when(
-((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 == 0 ~ 0L;
-((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt; 0 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 1 ~ 1L;
-((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 1 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 3 ~ 2L;
-((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 3 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 5 ~ 3L;
-((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 5 &amp; ((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &lt; 7 ~ 4L;
-((y8Q64atotmins*5) + (y8Q64btotmins*2)) / 7 / 60 &gt;= 7 ~ 5L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>y8Q119a</t>
   </si>
   <si>
@@ -1748,16 +1735,7 @@
 na.rm = TRUE)</t>
   </si>
   <si>
-    <t>hdl_chol</t>
-  </si>
-  <si>
     <t>ldl_chol</t>
-  </si>
-  <si>
-    <t>cholesterol ; hdl_chol ; Triglycerides</t>
-  </si>
-  <si>
-    <t>cholesterol - hdl_chol - (triglycerides/2.2)</t>
   </si>
   <si>
     <t>D1_sleepqual</t>
@@ -1801,11 +1779,33 @@
     <t>round(y8cesd10)</t>
   </si>
   <si>
+    <t>y8q64atotmins; y8q64btotmins</t>
+  </si>
+  <si>
     <t>round(rowSums(mutate(.,
-temp_y8Q64atotmins = y8Q64atotmins*5,
-temp_y8Q64btotmins = y8Q64btotmins*2) %&gt;%
-select(temp_y8Q64atotmins, temp_y8Q64btotmins),
+temp_y8q64atotmins = y8q64atotmins*5,
+temp_y8q64btotmins = y8q64btotmins*2) %&gt;%
+select(temp_y8q64atotmins, temp_y8q64btotmins),
 na.rm=TRUE) / 7 / 60)</t>
+  </si>
+  <si>
+    <t>case_when(
+((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 == 0 ~ 0L;
+((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt; 0 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 1 ~ 1L;
+((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 1 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 3 ~ 2L;
+((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 3 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 5 ~ 3L;
+((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 5 &amp; ((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &lt; 7 ~ 4L;
+((y8q64atotmins*5) + (y8q64btotmins*2)) / 7 / 60 &gt;= 7 ~ 5L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>hdl_Chol</t>
+  </si>
+  <si>
+    <t>cholesterol - hdl_Chol - (triglycerides/2.2)</t>
+  </si>
+  <si>
+    <t>cholesterol ; hdl_Chol ; Triglycerides</t>
   </si>
 </sst>
 </file>
@@ -2281,10 +2281,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P76" sqref="P76"/>
+      <selection pane="bottomRight" activeCell="T68" sqref="T68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -3992,7 +3992,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>340</v>
@@ -4045,7 +4045,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4072,7 +4072,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>364</v>
@@ -4778,7 +4778,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4830,7 +4830,7 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4934,7 +4934,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -5316,7 +5316,7 @@
         <v>34</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5626,19 +5626,19 @@
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="399" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5677,18 +5677,20 @@
       <c r="N68" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="O68" s="3"/>
+      <c r="O68" s="11" t="s">
+        <v>434</v>
+      </c>
       <c r="P68" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="S68" s="11" t="s">
-        <v>434</v>
+        <v>473</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
@@ -5716,7 +5718,7 @@
         <v>241</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>377</v>
@@ -6039,7 +6041,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="K76" s="3" t="s">
         <v>380</v>
@@ -6064,7 +6066,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6090,7 +6092,7 @@
         <v>267</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>380</v>
@@ -6115,7 +6117,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>463</v>
+        <v>483</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6143,7 +6145,7 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>394</v>
@@ -6164,7 +6166,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6237,7 +6239,7 @@
         <v>191</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K80" s="11" t="s">
         <v>395</v>
@@ -6260,7 +6262,7 @@
         <v>207</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6333,7 +6335,7 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>396</v>
@@ -6356,7 +6358,7 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6382,7 +6384,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K83" s="11" t="s">
         <v>397</v>
@@ -6403,7 +6405,7 @@
         <v>34</v>
       </c>
       <c r="S83" s="11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="84" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6431,7 +6433,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="8"/>
       <c r="J84" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>397</v>
@@ -6452,7 +6454,7 @@
         <v>34</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting variable names again
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5300495-6DAF-4721-B643-50EFAEB40EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCD12E-E0A1-4CD5-A2AA-4DE7E208D055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1577,9 +1577,6 @@
     <t>recode(1=1; 2=2; 3=3; 4=3; 5=3; 6=3; ELSE=NA)</t>
   </si>
   <si>
-    <t>recode(1=2; 2=1; 3=1; 4=1; 5=1; 6=1; 7=1; ELSE=NA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sleep duration. Average sleep duration in hours derived from sleep diary. A participant reported the time they felt asleep and the time they got out of bed for 8 days using the sleep diary. This variable represents the average sleep duration for these days days. 
 </t>
   </si>
@@ -1600,9 +1597,6 @@
   </si>
   <si>
     <t>y8Q127</t>
-  </si>
-  <si>
-    <t>y8Q65</t>
   </si>
   <si>
     <t>y8Q121</t>
@@ -1806,6 +1800,12 @@
   </si>
   <si>
     <t>cholesterol ; hdl_Chol ; Triglycerides</t>
+  </si>
+  <si>
+    <t>recode(1=2; 2=1; 3=1; 4=1; 5=1; 6=1; 7=1; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>y8ariapgp</t>
   </si>
 </sst>
 </file>
@@ -2281,10 +2281,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T68" sqref="T68"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>49</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>300</v>
@@ -2688,7 +2688,7 @@
         <v>60</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>303</v>
@@ -2711,7 +2711,7 @@
         <v>207</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="8"/>
       <c r="J11" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>305</v>
@@ -2921,7 +2921,7 @@
         <v>81</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>307</v>
@@ -2972,7 +2972,7 @@
         <v>85</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>307</v>
@@ -3023,7 +3023,7 @@
         <v>88</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>447</v>
+        <v>486</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>311</v>
@@ -3046,7 +3046,7 @@
         <v>40</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>440</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -3992,7 +3992,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>340</v>
@@ -4045,7 +4045,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4072,7 +4072,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="8"/>
       <c r="J38" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>349</v>
@@ -4251,7 +4251,7 @@
         <v>158</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>349</v>
@@ -4302,7 +4302,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
       <c r="J40" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>351</v>
@@ -4445,7 +4445,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="8"/>
       <c r="J43" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>353</v>
@@ -4496,7 +4496,7 @@
         <v>174</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>355</v>
@@ -4549,7 +4549,7 @@
         <v>178</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>358</v>
@@ -4600,7 +4600,7 @@
         <v>181</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>358</v>
@@ -4651,7 +4651,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="8"/>
       <c r="J47" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>362</v>
@@ -4674,7 +4674,7 @@
         <v>207</v>
       </c>
       <c r="S47" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>364</v>
@@ -4753,7 +4753,7 @@
         <v>191</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K49" s="11" t="s">
         <v>390</v>
@@ -4778,7 +4778,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>191</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K50" s="11" t="s">
         <v>391</v>
@@ -4830,7 +4830,7 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4858,7 +4858,7 @@
         <v>191</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>368</v>
@@ -4881,7 +4881,7 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4909,7 +4909,7 @@
         <v>200</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>368</v>
@@ -4934,7 +4934,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -4962,7 +4962,7 @@
         <v>191</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>392</v>
@@ -4985,7 +4985,7 @@
         <v>207</v>
       </c>
       <c r="S53" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>191</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>370</v>
@@ -5199,7 +5199,7 @@
         <v>191</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>438</v>
@@ -5316,7 +5316,7 @@
         <v>34</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5616,7 +5616,7 @@
         <v>375</v>
       </c>
       <c r="L67" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M67" s="8" t="s">
         <v>315</v>
@@ -5626,16 +5626,16 @@
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="399" x14ac:dyDescent="0.25">
@@ -5681,16 +5681,16 @@
         <v>434</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
@@ -5718,7 +5718,7 @@
         <v>241</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>377</v>
@@ -6041,7 +6041,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="K76" s="3" t="s">
         <v>380</v>
@@ -6066,7 +6066,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>267</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>380</v>
@@ -6117,7 +6117,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6145,7 +6145,7 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>394</v>
@@ -6166,7 +6166,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6239,7 +6239,7 @@
         <v>191</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K80" s="11" t="s">
         <v>395</v>
@@ -6262,7 +6262,7 @@
         <v>207</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6335,7 +6335,7 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>396</v>
@@ -6358,7 +6358,7 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6384,7 +6384,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K83" s="11" t="s">
         <v>397</v>
@@ -6405,7 +6405,7 @@
         <v>34</v>
       </c>
       <c r="S83" s="11" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="84" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6433,7 +6433,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="8"/>
       <c r="J84" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>397</v>
@@ -6454,7 +6454,7 @@
         <v>34</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update variable names again again
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCD12E-E0A1-4CD5-A2AA-4DE7E208D055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266E02B8-5745-4F62-BF71-D23F00BF0630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1649,16 +1649,6 @@
     <t>y8Q24m</t>
   </si>
   <si>
-    <t>y8Q119a</t>
-  </si>
-  <si>
-    <t>case_when(
-y8Q119a &gt; 1 ~ 1L;
-y8Q119a &lt;= 5 ~ 2L;
-y8Q119a &gt;= 6 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>y8Q120a;_x000D_
 y8Q120b</t>
   </si>
@@ -1667,21 +1657,6 @@
 y8Q120a == 1 ~1L;
 y8Q120b == 1 ~ 1L;
 (y8Q120a == 0) &amp; (y8Q120b == 0) ~ 0L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>y8Q119b; _x000D_
-y8Q119c;_x000D_
-y8Q120a;_x000D_
-y8Q120b</t>
-  </si>
-  <si>
-    <t>case_when(
-(y8Q119b == 0) &amp; (y8Q119c == 0) &amp; (y8Q120a== 0) &amp; (y8Q120b== 0) ~ 0L;
-!is.na(y8Q119b) ~ 1L; 
-!is.na(y8Q119c) ~ 1L;
-y8Q120a== 1 ~ 1L;
-y8Q120b== 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
@@ -1796,9 +1771,6 @@
     <t>hdl_Chol</t>
   </si>
   <si>
-    <t>cholesterol - hdl_Chol - (triglycerides/2.2)</t>
-  </si>
-  <si>
     <t>cholesterol ; hdl_Chol ; Triglycerides</t>
   </si>
   <si>
@@ -1806,6 +1778,34 @@
   </si>
   <si>
     <t>y8ariapgp</t>
+  </si>
+  <si>
+    <t>cholesterol - hdl_Chol - (Triglycerides/2.2)</t>
+  </si>
+  <si>
+    <t>y8q119b; 
+y8q119c;
+y8Q120a;
+y8Q120b</t>
+  </si>
+  <si>
+    <t>y8q119a</t>
+  </si>
+  <si>
+    <t>case_when(
+y8q119a &gt; 1 ~ 1L;
+y8q119a &lt;= 5 ~ 2L;
+y8q119a &gt;= 6 ~ 3L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+(y8q119b == 0) &amp; (y8q119c == 0) &amp; (y8Q120a== 0) &amp; (y8Q120b== 0) ~ 0L;
+!is.na(y8q119b) ~ 1L; 
+!is.na(y8q119c) ~ 1L;
+y8Q120a== 1 ~ 1L;
+y8Q120b== 1 ~ 1L;
+ELSE ~ NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -2281,10 +2281,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>88</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>311</v>
@@ -3046,7 +3046,7 @@
         <v>40</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -3992,7 +3992,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>340</v>
@@ -4045,7 +4045,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4072,7 +4072,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>364</v>
@@ -4778,7 +4778,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4830,7 +4830,7 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4881,7 +4881,7 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4934,7 +4934,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -5316,7 +5316,7 @@
         <v>34</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5626,16 +5626,16 @@
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="399" x14ac:dyDescent="0.25">
@@ -5681,16 +5681,16 @@
         <v>434</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
@@ -5718,7 +5718,7 @@
         <v>241</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>377</v>
@@ -6041,7 +6041,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="K76" s="3" t="s">
         <v>380</v>
@@ -6066,7 +6066,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>267</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>380</v>
@@ -6117,7 +6117,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6145,7 +6145,7 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>460</v>
+        <v>484</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>394</v>
@@ -6166,7 +6166,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>461</v>
+        <v>485</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6239,7 +6239,7 @@
         <v>191</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K80" s="11" t="s">
         <v>395</v>
@@ -6262,7 +6262,7 @@
         <v>207</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6335,7 +6335,7 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>464</v>
+        <v>483</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>396</v>
@@ -6358,7 +6358,7 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>465</v>
+        <v>486</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6384,7 +6384,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="K83" s="11" t="s">
         <v>397</v>
@@ -6405,7 +6405,7 @@
         <v>34</v>
       </c>
       <c r="S83" s="11" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="84" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6433,7 +6433,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="8"/>
       <c r="J84" s="11" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>397</v>
@@ -6454,7 +6454,7 @@
         <v>34</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct fruit frequency AWH
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266E02B8-5745-4F62-BF71-D23F00BF0630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7262B980-4D1E-48E0-99E0-87B82C04D451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1574,9 +1574,6 @@
     <t>Self-reported Depression</t>
   </si>
   <si>
-    <t>recode(1=1; 2=2; 3=3; 4=3; 5=3; 6=3; ELSE=NA)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sleep duration. Average sleep duration in hours derived from sleep diary. A participant reported the time they felt asleep and the time they got out of bed for 8 days using the sleep diary. This variable represents the average sleep duration for these days days. 
 </t>
   </si>
@@ -1806,6 +1803,9 @@
 y8Q120a== 1 ~ 1L;
 y8Q120b== 1 ~ 1L;
 ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>recode(1=1; 2=NA; 3=3; 4=3; 5=3; 6=3; ELSE=NA)</t>
   </si>
 </sst>
 </file>
@@ -2281,10 +2281,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>49</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>300</v>
@@ -2688,7 +2688,7 @@
         <v>60</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>303</v>
@@ -2711,7 +2711,7 @@
         <v>207</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="8"/>
       <c r="J11" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>305</v>
@@ -2921,7 +2921,7 @@
         <v>81</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>307</v>
@@ -2972,7 +2972,7 @@
         <v>85</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>307</v>
@@ -3023,7 +3023,7 @@
         <v>88</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>311</v>
@@ -3046,7 +3046,7 @@
         <v>40</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3939,7 +3939,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -3992,7 +3992,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>340</v>
@@ -4045,7 +4045,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4072,7 +4072,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="8"/>
       <c r="J38" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>349</v>
@@ -4251,7 +4251,7 @@
         <v>158</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>349</v>
@@ -4274,7 +4274,7 @@
         <v>40</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>439</v>
+        <v>486</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="157.5" x14ac:dyDescent="0.25">
@@ -4302,7 +4302,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
       <c r="J40" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>351</v>
@@ -4445,7 +4445,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="8"/>
       <c r="J43" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>353</v>
@@ -4496,7 +4496,7 @@
         <v>174</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>355</v>
@@ -4549,7 +4549,7 @@
         <v>178</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>358</v>
@@ -4600,7 +4600,7 @@
         <v>181</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>358</v>
@@ -4651,7 +4651,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="8"/>
       <c r="J47" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>362</v>
@@ -4674,7 +4674,7 @@
         <v>207</v>
       </c>
       <c r="S47" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>364</v>
@@ -4753,7 +4753,7 @@
         <v>191</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K49" s="11" t="s">
         <v>390</v>
@@ -4778,7 +4778,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>191</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K50" s="11" t="s">
         <v>391</v>
@@ -4830,7 +4830,7 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4858,7 +4858,7 @@
         <v>191</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>368</v>
@@ -4881,7 +4881,7 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4909,7 +4909,7 @@
         <v>200</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>368</v>
@@ -4934,7 +4934,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -4962,7 +4962,7 @@
         <v>191</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K53" s="3" t="s">
         <v>392</v>
@@ -4985,7 +4985,7 @@
         <v>207</v>
       </c>
       <c r="S53" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>191</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>370</v>
@@ -5199,7 +5199,7 @@
         <v>191</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>438</v>
@@ -5316,7 +5316,7 @@
         <v>34</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5616,7 +5616,7 @@
         <v>375</v>
       </c>
       <c r="L67" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M67" s="8" t="s">
         <v>315</v>
@@ -5626,16 +5626,16 @@
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="399" x14ac:dyDescent="0.25">
@@ -5681,16 +5681,16 @@
         <v>434</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
@@ -5718,7 +5718,7 @@
         <v>241</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>377</v>
@@ -6041,7 +6041,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K76" s="3" t="s">
         <v>380</v>
@@ -6066,7 +6066,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>267</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>380</v>
@@ -6117,7 +6117,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6145,7 +6145,7 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>394</v>
@@ -6166,7 +6166,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6239,7 +6239,7 @@
         <v>191</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K80" s="11" t="s">
         <v>395</v>
@@ -6262,7 +6262,7 @@
         <v>207</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6335,7 +6335,7 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>396</v>
@@ -6358,7 +6358,7 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6384,7 +6384,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="8"/>
       <c r="J83" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K83" s="11" t="s">
         <v>397</v>
@@ -6405,7 +6405,7 @@
         <v>34</v>
       </c>
       <c r="S83" s="11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="84" spans="1:19" ht="285" x14ac:dyDescent="0.25">
@@ -6433,7 +6433,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="8"/>
       <c r="J84" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K84" s="11" t="s">
         <v>397</v>
@@ -6454,7 +6454,7 @@
         <v>34</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the sleep duration variable
</commit_message>
<xml_diff>
--- a/data_processing_elements-AWH.xlsx
+++ b/data_processing_elements-AWH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7262B980-4D1E-48E0-99E0-87B82C04D451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB833AAF-FFCD-409D-B763-94EE9EFCB596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="487">
   <si>
     <t>index</t>
   </si>
@@ -1707,9 +1707,6 @@
     <t>D1_sleepqual</t>
   </si>
   <si>
-    <t>undetermined</t>
-  </si>
-  <si>
     <t>y8sf</t>
   </si>
   <si>
@@ -1806,6 +1803,9 @@
   </si>
   <si>
     <t>recode(1=1; 2=NA; 3=3; 4=3; 5=3; 6=3; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>sleep_duration_hours</t>
   </si>
 </sst>
 </file>
@@ -1853,7 +1853,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1875,12 +1875,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC99FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1936,7 +1930,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2281,10 +2275,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
+      <selection pane="bottomRight" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2558,7 @@
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="102" x14ac:dyDescent="0.25">
@@ -3023,7 +3017,7 @@
         <v>88</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>311</v>
@@ -3046,7 +3040,7 @@
         <v>40</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3939,7 +3933,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>338</v>
@@ -4045,7 +4039,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>342</v>
@@ -4072,7 +4066,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4190,7 +4184,7 @@
         <v>152</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>153</v>
@@ -4274,7 +4268,7 @@
         <v>40</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="157.5" x14ac:dyDescent="0.25">
@@ -4294,7 +4288,7 @@
         <v>161</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>153</v>
@@ -4702,7 +4696,7 @@
         <v>187</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>364</v>
@@ -4778,7 +4772,7 @@
         <v>207</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
@@ -4830,7 +4824,7 @@
         <v>207</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4881,7 +4875,7 @@
         <v>207</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -4934,7 +4928,7 @@
         <v>207</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="270.75" x14ac:dyDescent="0.25">
@@ -5316,7 +5310,7 @@
         <v>34</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -5610,7 +5604,7 @@
       <c r="H67" s="3"/>
       <c r="I67" s="8"/>
       <c r="J67" s="14" t="s">
-        <v>55</v>
+        <v>486</v>
       </c>
       <c r="K67" s="3" t="s">
         <v>375</v>
@@ -5626,19 +5620,19 @@
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
-        <v>466</v>
+        <v>25</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>466</v>
+        <v>26</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>466</v>
+        <v>45</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="399" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5663,7 +5657,7 @@
         <v>238</v>
       </c>
       <c r="J68" s="14" t="s">
-        <v>55</v>
+        <v>486</v>
       </c>
       <c r="K68" s="3" t="s">
         <v>375</v>
@@ -5677,20 +5671,17 @@
       <c r="N68" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="O68" s="11" t="s">
+      <c r="P68" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="S68" s="11" t="s">
         <v>434</v>
-      </c>
-      <c r="P68" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="Q68" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="R68" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="S68" s="3" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
@@ -6041,7 +6032,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="8"/>
       <c r="J76" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K76" s="3" t="s">
         <v>380</v>
@@ -6066,7 +6057,7 @@
         <v>34</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
@@ -6092,7 +6083,7 @@
         <v>267</v>
       </c>
       <c r="J77" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>380</v>
@@ -6117,7 +6108,7 @@
         <v>207</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="342" x14ac:dyDescent="0.25">
@@ -6145,7 +6136,7 @@
         <v>271</v>
       </c>
       <c r="J78" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K78" s="11" t="s">
         <v>394</v>
@@ -6166,7 +6157,7 @@
         <v>207</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -6335,7 +6326,7 @@
         <v>191</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K82" s="11" t="s">
         <v>396</v>
@@ -6358,7 +6349,7 @@
         <v>207</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="83" spans="1:19" ht="285" x14ac:dyDescent="0.25">

</xml_diff>